<commit_message>
Remove col "Versorgungsfall (Aufnahmegrund)"
The column "Versorgungsfall (Aufnahmegrund)" in the table sheet "Versorgungsfall" in the convertable Excel files is now removed. All diagnoses entered there in the test data Excel files were transferred to the "Diagnosen" spreadsheet and explicitly marked as admission diagnoses. This also means that the admission diagnoses in Encounter always have a correct reference to the condition with the corresponding diagnosis code and date.
</commit_message>
<xml_diff>
--- a/src/main/resources/excel/POLAR_Testdaten_UKT.xlsx
+++ b/src/main/resources/excel/POLAR_Testdaten_UKT.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Eigene Projekte\smith\TestDataGenerator\src\main\resources\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EDFFB72-90BE-4FAB-BAF7-4B91B61EA183}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9001402-ED80-442A-8825-BBC58130D14C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="23640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="8400" windowWidth="4755" windowHeight="3465" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Person" sheetId="2" r:id="rId1"/>
@@ -887,18 +887,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="67" customWidth="1"/>
+    <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.140625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="13.42578125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="20.85546875" customWidth="1"/>
   </cols>
@@ -996,12 +996,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="22" bestFit="1" customWidth="1"/>
@@ -2285,27 +2286,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_dlc_DocId xmlns="15b42a90-06dd-4669-ae82-892e5974bb2f">TMFEV-111023110-969</_dlc_DocId>
-    <_dlc_DocIdUrl xmlns="15b42a90-06dd-4669-ae82-892e5974bb2f">
-      <Url>https://tmfev.sharepoint.com/sites/tmf/mi-i/_layouts/15/DocIdRedir.aspx?ID=TMFEV-111023110-969</Url>
-      <Description>TMFEV-111023110-969</Description>
-    </_dlc_DocIdUrl>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
   <Receiver>
@@ -2355,6 +2335,27 @@
 </spe:Receivers>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_dlc_DocId xmlns="15b42a90-06dd-4669-ae82-892e5974bb2f">TMFEV-111023110-969</_dlc_DocId>
+    <_dlc_DocIdUrl xmlns="15b42a90-06dd-4669-ae82-892e5974bb2f">
+      <Url>https://tmfev.sharepoint.com/sites/tmf/mi-i/_layouts/15/DocIdRedir.aspx?ID=TMFEV-111023110-969</Url>
+      <Description>TMFEV-111023110-969</Description>
+    </_dlc_DocIdUrl>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6E73BDE1-9CCD-4DA3-98C1-B2700F42483C}">
   <ds:schemaRefs>
@@ -2376,11 +2377,9 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1B89C2DA-DD1E-4298-9623-BC864CA91962}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{17381246-8561-41AA-90B8-1B77E21DFFC0}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="15b42a90-06dd-4669-ae82-892e5974bb2f"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -2394,9 +2393,11 @@
 </file>
 
 <file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{17381246-8561-41AA-90B8-1B77E21DFFC0}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1B89C2DA-DD1E-4298-9623-BC864CA91962}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="15b42a90-06dd-4669-ae82-892e5974bb2f"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Unform PIDs and (still empty) Consent columns in all Excel files
</commit_message>
<xml_diff>
--- a/src/main/resources/excel/POLAR_Testdaten_UKT.xlsx
+++ b/src/main/resources/excel/POLAR_Testdaten_UKT.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24729"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Eigene Projekte\smith\TestDataGenerator\src\main\resources\excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Eigene Projekte\smith\TestDataGenerator\input - Vorlagen\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9001402-ED80-442A-8825-BBC58130D14C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{730755F8-FBDB-490D-868E-1AE96ECAB6E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="8400" windowWidth="4755" windowHeight="3465" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3810" yWindow="3810" windowWidth="28800" windowHeight="17235" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Person" sheetId="2" r:id="rId1"/>
@@ -51,9 +51,6 @@
     <t>Krankenkasse</t>
   </si>
   <si>
-    <t>UKT001</t>
-  </si>
-  <si>
     <t>Grete</t>
   </si>
   <si>
@@ -66,9 +63,6 @@
     <t>AOK</t>
   </si>
   <si>
-    <t>UKT002</t>
-  </si>
-  <si>
     <t>Hans</t>
   </si>
   <si>
@@ -81,9 +75,6 @@
     <t>TKK</t>
   </si>
   <si>
-    <t>UKT003</t>
-  </si>
-  <si>
     <t>Karla</t>
   </si>
   <si>
@@ -385,6 +376,15 @@
   </si>
   <si>
     <t>Zeitstempel (Abnahme)</t>
+  </si>
+  <si>
+    <t>UKT_0001</t>
+  </si>
+  <si>
+    <t>UKT_0002</t>
+  </si>
+  <si>
+    <t>UKT_0003</t>
   </si>
 </sst>
 </file>
@@ -888,7 +888,7 @@
   <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -928,62 +928,62 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>116</v>
+      </c>
+      <c r="B2" t="s">
         <v>7</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>8</v>
-      </c>
-      <c r="C2" t="s">
-        <v>9</v>
       </c>
       <c r="E2" s="4">
         <v>23360</v>
       </c>
       <c r="F2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G2" t="s">
         <v>10</v>
-      </c>
-      <c r="G2" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>117</v>
+      </c>
+      <c r="B3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" t="s">
         <v>12</v>
-      </c>
-      <c r="B3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C3" t="s">
-        <v>14</v>
       </c>
       <c r="E3" s="12">
         <v>17020</v>
       </c>
       <c r="F3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="G3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>17</v>
+        <v>118</v>
       </c>
       <c r="B4" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C4" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="E4" s="4">
         <v>11230</v>
       </c>
       <c r="F4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G4" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -996,7 +996,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -1013,16 +1013,16 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>21</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -1035,7 +1035,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1051,18 +1051,18 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>22</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>7</v>
+        <v>116</v>
       </c>
       <c r="B2" s="4">
         <v>43924</v>
@@ -1071,23 +1071,23 @@
         <v>43925</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>12</v>
+        <v>117</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>17</v>
+        <v>118</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -1100,7 +1100,7 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1116,89 +1116,89 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>27</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>7</v>
+        <v>116</v>
       </c>
       <c r="B2" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="F2" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>116</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="F3" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>12</v>
+        <v>117</v>
       </c>
       <c r="B4" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="F4" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>17</v>
+        <v>118</v>
       </c>
       <c r="B5" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C5" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="F5" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>17</v>
+        <v>118</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="F6" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -1211,7 +1211,7 @@
   <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1226,103 +1226,103 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C1" s="14" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>7</v>
+        <v>116</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C2" s="15" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>12</v>
+        <v>117</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C3" s="15" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>17</v>
+        <v>118</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C4" s="15" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>7</v>
+        <v>116</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C5" s="15" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>12</v>
+        <v>117</v>
       </c>
       <c r="B6" s="13" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C6" s="15" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>17</v>
+        <v>118</v>
       </c>
       <c r="B7" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="C7" s="15" t="s">
         <v>49</v>
-      </c>
-      <c r="C7" s="15" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>7</v>
+        <v>116</v>
       </c>
       <c r="B8" s="17" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C8" s="18" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="D8" s="19"/>
       <c r="E8" s="19"/>
     </row>
     <row r="9" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>12</v>
+        <v>117</v>
       </c>
       <c r="B9" s="17" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C9" s="18" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="10" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -1362,22 +1362,22 @@
   <sheetData>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B3" t="s">
+        <v>53</v>
+      </c>
+      <c r="C3" t="s">
+        <v>54</v>
+      </c>
+      <c r="D3" t="s">
         <v>55</v>
       </c>
-      <c r="B3" t="s">
+      <c r="E3" t="s">
         <v>56</v>
       </c>
-      <c r="C3" t="s">
+      <c r="F3" t="s">
         <v>57</v>
-      </c>
-      <c r="D3" t="s">
-        <v>58</v>
-      </c>
-      <c r="E3" t="s">
-        <v>59</v>
-      </c>
-      <c r="F3" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -1385,48 +1385,48 @@
         <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C4" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>61</v>
+      </c>
+      <c r="B6" t="s">
+        <v>62</v>
+      </c>
+      <c r="C6" t="s">
+        <v>63</v>
+      </c>
+      <c r="D6" t="s">
         <v>64</v>
       </c>
-      <c r="B6" t="s">
+      <c r="E6" t="s">
         <v>65</v>
-      </c>
-      <c r="C6" t="s">
-        <v>66</v>
-      </c>
-      <c r="D6" t="s">
-        <v>67</v>
-      </c>
-      <c r="E6" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
   </sheetData>
@@ -1442,9 +1442,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:R16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1464,54 +1462,54 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="G1" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>81</v>
-      </c>
       <c r="I1" s="1" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>7</v>
+        <v>116</v>
       </c>
       <c r="C2" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="F2" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="G2" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="I2" s="9">
         <v>5.9</v>
       </c>
       <c r="J2" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="K2" s="10">
         <v>42703</v>
@@ -1519,22 +1517,22 @@
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>116</v>
       </c>
       <c r="C3" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="F3" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="G3" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="I3" s="9">
         <v>1.5</v>
       </c>
       <c r="J3" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="K3" s="10">
         <v>42703</v>
@@ -1543,22 +1541,22 @@
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>116</v>
       </c>
       <c r="C4" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="F4" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="G4" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="I4" s="9">
         <v>46.5</v>
       </c>
       <c r="J4" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="K4" s="10">
         <v>42703</v>
@@ -1566,22 +1564,22 @@
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>12</v>
+        <v>117</v>
       </c>
       <c r="C5" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="F5" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="G5" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="I5" s="9">
         <v>9.6999999999999993</v>
       </c>
       <c r="J5" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="K5" s="10">
         <v>42765</v>
@@ -1589,22 +1587,22 @@
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>12</v>
+        <v>117</v>
       </c>
       <c r="C6" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="F6" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="G6" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="I6" s="9">
         <v>0.7</v>
       </c>
       <c r="J6" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="K6" s="10">
         <v>42765</v>
@@ -1615,22 +1613,22 @@
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>12</v>
+        <v>117</v>
       </c>
       <c r="C7" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="F7" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="G7" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="I7" s="9">
         <v>99.24</v>
       </c>
       <c r="J7" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="K7" s="10">
         <v>42765</v>
@@ -1638,22 +1636,22 @@
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>17</v>
+        <v>118</v>
       </c>
       <c r="C8" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="F8" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="G8" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="I8" s="9">
         <v>11.5</v>
       </c>
       <c r="J8" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="K8" s="10">
         <v>42982</v>
@@ -1661,26 +1659,26 @@
     </row>
     <row r="9" spans="1:18" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>17</v>
+        <v>118</v>
       </c>
       <c r="B9"/>
       <c r="C9" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="D9"/>
       <c r="E9"/>
       <c r="F9" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="G9" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="H9"/>
       <c r="I9" s="9">
         <v>1.1000000000000001</v>
       </c>
       <c r="J9" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="K9" s="10">
         <v>42982</v>
@@ -1691,26 +1689,26 @@
     </row>
     <row r="10" spans="1:18" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>17</v>
+        <v>118</v>
       </c>
       <c r="B10"/>
       <c r="C10" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="D10"/>
       <c r="E10"/>
       <c r="F10" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="G10" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="H10"/>
       <c r="I10" s="9">
         <v>60.04</v>
       </c>
       <c r="J10" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="K10" s="10">
         <v>42982</v>
@@ -1743,7 +1741,7 @@
   <dimension ref="A1:M28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1765,57 +1763,57 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="J1" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>96</v>
-      </c>
       <c r="M1" s="1" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>7</v>
+        <v>116</v>
       </c>
       <c r="B2" s="10">
         <v>42703</v>
       </c>
       <c r="C2" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="D2" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="G2" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="I2">
         <v>1</v>
@@ -1824,24 +1822,24 @@
         <v>75</v>
       </c>
       <c r="M2" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>116</v>
       </c>
       <c r="B3" s="10">
         <v>42703</v>
       </c>
       <c r="C3" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="D3" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="G3" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="I3">
         <v>1</v>
@@ -1850,24 +1848,24 @@
         <v>100</v>
       </c>
       <c r="M3" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>12</v>
+        <v>117</v>
       </c>
       <c r="B4" s="10">
         <v>42765</v>
       </c>
       <c r="C4" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="D4" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="G4" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="I4">
         <v>1</v>
@@ -1876,24 +1874,24 @@
         <v>6</v>
       </c>
       <c r="M4" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>17</v>
+        <v>118</v>
       </c>
       <c r="B5" s="10">
         <v>42982</v>
       </c>
       <c r="C5" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="D5" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="G5" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="I5">
         <v>1</v>
@@ -1902,7 +1900,7 @@
         <v>9</v>
       </c>
       <c r="M5" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="21" spans="3:3" x14ac:dyDescent="0.25">
@@ -1950,7 +1948,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:F9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -1966,77 +1964,77 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>73</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="C2" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="E2" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="C3" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="E3" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="C4" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="E4" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
     </row>
   </sheetData>
@@ -2045,6 +2043,65 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10001</Type>
+    <SequenceNumber>1000</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10002</Type>
+    <SequenceNumber>1001</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10004</Type>
+    <SequenceNumber>1002</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10006</Type>
+    <SequenceNumber>1003</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+</spe:Receivers>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x010100DBF8EC412D8CCF4EB717AD3D944049CF" ma:contentTypeVersion="11" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="df242df24ce9c459e95a399f1d5f10f4">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="15b42a90-06dd-4669-ae82-892e5974bb2f" xmlns:ns3="2d89f73c-94c0-4155-aa8d-969ee56d6579" xmlns:ns4="eaa21d2e-573b-4747-938a-ffc27391051f" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="9eb0b91dce5f86d4b3092630ff7b2144" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="15b42a90-06dd-4669-ae82-892e5974bb2f"/>
@@ -2285,65 +2342,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10001</Type>
-    <SequenceNumber>1000</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10002</Type>
-    <SequenceNumber>1001</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10004</Type>
-    <SequenceNumber>1002</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10006</Type>
-    <SequenceNumber>1003</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-</spe:Receivers>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -2357,6 +2355,22 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9F3EECB9-8F76-4A0D-B25B-69509DED7146}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{17381246-8561-41AA-90B8-1B77E21DFFC0}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6E73BDE1-9CCD-4DA3-98C1-B2700F42483C}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2376,22 +2390,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{17381246-8561-41AA-90B8-1B77E21DFFC0}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9F3EECB9-8F76-4A0D-B25B-69509DED7146}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1B89C2DA-DD1E-4298-9623-BC864CA91962}">
   <ds:schemaRefs>

</xml_diff>